<commit_message>
Version Nov 10, 2021
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/evaluation_output.xlsx
+++ b/data_driven/modeling/output/evaluation_output.xlsx
@@ -37,52 +37,52 @@
     <t xml:space="preserve">Model</t>
   </si>
   <si>
+    <t xml:space="preserve">Cross-validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are chemical groups included?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method for grouping chemicals in groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method for handling flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If applied, what is the number of intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method for encoding  industry sectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are the outliers removed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the dataset balanced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If applied, what is the method applied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is a method for dimensionality reduction applied?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If applied, what method is applied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the database split in a balanced way?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the data before 2005 included?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Validation</t>
   </si>
   <si>
-    <t xml:space="preserve">Are chemical groups included?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method for grouping chemicals in groups</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method for handling flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If applied, what is the number of intervals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method for encoding  industry sectors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output column</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are the outliers removed?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the dataset balanced?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If applied, what is the method applied</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is a method for dimensionality reduction applied?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If applied, what method is applied</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the database split in a balanced way?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the data before 2005 included?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External</t>
+    <t xml:space="preserve">Train</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -155,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -183,11 +183,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -264,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,7 +284,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,15 +300,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,14 +388,15 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="T10" activeCellId="0" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="45.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="23" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -465,7 +453,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="58.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1038,7 +1026,7 @@
       <c r="F13" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="5" t="s">
@@ -1074,7 +1062,7 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>11</v>
       </c>
@@ -1125,7 +1113,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>12</v>
       </c>
@@ -1176,7 +1164,7 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>13</v>
       </c>
@@ -1223,7 +1211,7 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>14</v>
       </c>
@@ -1268,7 +1256,7 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>15</v>
       </c>
@@ -1313,7 +1301,7 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>16</v>
       </c>
@@ -1358,7 +1346,7 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>17</v>
       </c>
@@ -1403,7 +1391,7 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>18</v>
       </c>
@@ -1431,7 +1419,7 @@
       <c r="M21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N21" s="12" t="s">
+      <c r="N21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="O21" s="7" t="s">
@@ -1446,7 +1434,7 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>19</v>
       </c>
@@ -1489,7 +1477,7 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>20</v>
       </c>
@@ -1532,7 +1520,7 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>21</v>
       </c>
@@ -1557,7 +1545,7 @@
         <v>26</v>
       </c>
       <c r="L24" s="9"/>
-      <c r="M24" s="13"/>
+      <c r="M24" s="11"/>
       <c r="N24" s="9"/>
       <c r="O24" s="7" t="s">
         <v>26</v>
@@ -1571,7 +1559,7 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>22</v>
       </c>
@@ -1596,7 +1584,7 @@
         <v>26</v>
       </c>
       <c r="L25" s="9"/>
-      <c r="M25" s="13"/>
+      <c r="M25" s="11"/>
       <c r="N25" s="9"/>
       <c r="O25" s="7" t="s">
         <v>26</v>
@@ -1610,7 +1598,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>23</v>
       </c>
@@ -1635,7 +1623,7 @@
         <v>26</v>
       </c>
       <c r="L26" s="9"/>
-      <c r="M26" s="13"/>
+      <c r="M26" s="11"/>
       <c r="N26" s="9"/>
       <c r="O26" s="7" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Version Nov 11, 2021
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/evaluation_output.xlsx
+++ b/data_driven/modeling/output/evaluation_output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="47">
   <si>
     <t xml:space="preserve">Identification ID</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t xml:space="preserve">Scores analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Running time (seg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data volume (GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -392,17 +404,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W26"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T7" activeCellId="0" sqref="T7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X7" activeCellId="0" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="45.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="24" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="45.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="28" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -438,6 +450,10 @@
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -460,6 +476,10 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
@@ -514,79 +534,95 @@
       <c r="T3" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F4" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
       <c r="T4" s="8"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>1</v>
@@ -595,58 +631,62 @@
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="8"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>2</v>
@@ -655,58 +695,62 @@
         <v>1</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="8"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>3</v>
@@ -715,54 +759,58 @@
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>4</v>
@@ -771,54 +819,58 @@
         <v>1</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>5</v>
@@ -827,54 +879,58 @@
         <v>1</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="8"/>
-    </row>
-    <row r="10" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>6</v>
@@ -883,54 +939,58 @@
         <v>1</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>7</v>
@@ -939,54 +999,58 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>8</v>
@@ -995,48 +1059,52 @@
         <v>1</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>2</v>
@@ -1047,48 +1115,52 @@
         <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>2</v>
@@ -1102,45 +1174,49 @@
         <v>10</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>2</v>
@@ -1154,45 +1230,49 @@
         <v>10</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>3</v>
@@ -1202,45 +1282,49 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>4</v>
@@ -1251,42 +1335,46 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="8"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>4</v>
@@ -1297,42 +1385,46 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="8"/>
-    </row>
-    <row r="19" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>4</v>
@@ -1343,42 +1435,46 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>4</v>
@@ -1389,42 +1485,46 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="8"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>5</v>
@@ -1435,40 +1535,44 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
       <c r="T21" s="8"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>5</v>
@@ -1479,40 +1583,44 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="8"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>5</v>
@@ -1523,40 +1631,44 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>6</v>
@@ -1567,36 +1679,40 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="12"/>
       <c r="N24" s="10"/>
       <c r="O24" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="8"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4" t="n">
         <v>6</v>
@@ -1607,36 +1723,40 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L25" s="10"/>
       <c r="M25" s="12"/>
       <c r="N25" s="10"/>
       <c r="O25" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25" s="8"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C26" s="4" t="n">
         <v>6</v>
@@ -1647,29 +1767,33 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L26" s="10"/>
       <c r="M26" s="12"/>
       <c r="N26" s="10"/>
       <c r="O26" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1678,7 +1802,7 @@
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:P2"/>
     <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="R1:T2"/>
+    <mergeCell ref="R1:X2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Version Nov 16, 2021
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/evaluation_output.xlsx
+++ b/data_driven/modeling/output/evaluation_output.xlsx
@@ -16,8 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -51,6 +53,11 @@
       <charset val="1"/>
       <family val="2"/>
       <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -169,15 +176,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -197,11 +201,14 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -227,6 +234,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -590,21 +603,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AI25"/>
+  <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="O1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V24" activeCellId="0" sqref="V24"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="9" min="1" max="19"/>
-    <col width="37.16" customWidth="1" style="9" min="20" max="20"/>
-    <col width="13.89" customWidth="1" style="9" min="21" max="21"/>
-    <col width="11.52" customWidth="1" style="9" min="22" max="32"/>
-    <col width="45.71" customWidth="1" style="9" min="33" max="33"/>
-    <col width="11.52" customWidth="1" style="9" min="34" max="1023"/>
-    <col width="11.52" customWidth="1" style="10" min="1024" max="1025"/>
+    <col width="11.52" customWidth="1" style="10" min="1" max="19"/>
+    <col width="37.16" customWidth="1" style="10" min="20" max="20"/>
+    <col width="13.89" customWidth="1" style="10" min="21" max="21"/>
+    <col width="11.52" customWidth="1" style="10" min="22" max="32"/>
+    <col width="45.71" customWidth="1" style="10" min="33" max="33"/>
+    <col width="11.52" customWidth="1" style="10" min="34" max="1025"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="11">
@@ -1811,8 +1823,10 @@
       <c r="C12" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="D12" s="24" t="b">
-        <v>1</v>
+      <c r="D12" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E12" s="24" t="n">
         <v>7</v>
@@ -1927,8 +1941,10 @@
       <c r="C13" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="D13" s="24" t="b">
-        <v>1</v>
+      <c r="D13" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E13" s="24" t="n">
         <v>7</v>
@@ -2041,8 +2057,10 @@
       <c r="C14" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="24" t="b">
-        <v>1</v>
+      <c r="D14" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E14" s="24" t="n">
         <v>7</v>
@@ -2155,8 +2173,10 @@
       <c r="C15" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="24" t="b">
-        <v>1</v>
+      <c r="D15" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E15" s="24" t="n">
         <v>7</v>
@@ -2259,7 +2279,7 @@
       </c>
       <c r="AD15" s="15" t="n"/>
     </row>
-    <row r="16" ht="12.8" customHeight="1" s="11">
+    <row r="16" ht="23.75" customHeight="1" s="11">
       <c r="A16" s="15" t="n">
         <v>13</v>
       </c>
@@ -2271,8 +2291,10 @@
       <c r="C16" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D16" s="24" t="b">
-        <v>1</v>
+      <c r="D16" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E16" s="24" t="n">
         <v>7</v>
@@ -2375,7 +2397,7 @@
       </c>
       <c r="AD16" s="15" t="n"/>
     </row>
-    <row r="17" ht="12.8" customHeight="1" s="11">
+    <row r="17" ht="23.75" customHeight="1" s="11">
       <c r="A17" s="15" t="n">
         <v>14</v>
       </c>
@@ -2387,8 +2409,10 @@
       <c r="C17" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="24" t="b">
-        <v>1</v>
+      <c r="D17" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E17" s="24" t="n">
         <v>7</v>
@@ -2491,7 +2515,7 @@
       </c>
       <c r="AD17" s="15" t="n"/>
     </row>
-    <row r="18" ht="23.85" customHeight="1" s="11">
+    <row r="18" ht="23.75" customHeight="1" s="11">
       <c r="A18" s="15" t="n">
         <v>15</v>
       </c>
@@ -2503,8 +2527,10 @@
       <c r="C18" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D18" s="24" t="b">
-        <v>1</v>
+      <c r="D18" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E18" s="24" t="n">
         <v>7</v>
@@ -2607,7 +2633,7 @@
       </c>
       <c r="AD18" s="15" t="n"/>
     </row>
-    <row r="19" ht="12.8" customHeight="1" s="11">
+    <row r="19" ht="23.75" customHeight="1" s="11">
       <c r="A19" s="15" t="n">
         <v>16</v>
       </c>
@@ -2619,8 +2645,10 @@
       <c r="C19" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="24" t="b">
-        <v>1</v>
+      <c r="D19" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E19" s="24" t="n">
         <v>7</v>
@@ -2723,7 +2751,7 @@
       </c>
       <c r="AD19" s="15" t="n"/>
     </row>
-    <row r="20" ht="12.8" customHeight="1" s="11">
+    <row r="20" ht="23.75" customHeight="1" s="11">
       <c r="A20" s="15" t="n">
         <v>17</v>
       </c>
@@ -2735,8 +2763,10 @@
       <c r="C20" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D20" s="24" t="b">
-        <v>1</v>
+      <c r="D20" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E20" s="24" t="n">
         <v>7</v>
@@ -2839,7 +2869,7 @@
       </c>
       <c r="AD20" s="15" t="n"/>
     </row>
-    <row r="21" ht="12.8" customHeight="1" s="11">
+    <row r="21" ht="23.75" customHeight="1" s="11">
       <c r="A21" s="15" t="n">
         <v>18</v>
       </c>
@@ -2851,8 +2881,10 @@
       <c r="C21" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D21" s="24" t="b">
-        <v>1</v>
+      <c r="D21" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E21" s="24" t="n">
         <v>7</v>
@@ -2955,7 +2987,7 @@
       </c>
       <c r="AD21" s="15" t="n"/>
     </row>
-    <row r="22" ht="12.8" customHeight="1" s="11">
+    <row r="22" ht="23.75" customHeight="1" s="11">
       <c r="A22" s="15" t="n">
         <v>19</v>
       </c>
@@ -2967,8 +2999,10 @@
       <c r="C22" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="D22" s="24" t="b">
-        <v>1</v>
+      <c r="D22" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E22" s="24" t="n">
         <v>7</v>
@@ -3071,7 +3105,7 @@
       </c>
       <c r="AD22" s="15" t="n"/>
     </row>
-    <row r="23" ht="12.8" customHeight="1" s="11">
+    <row r="23" ht="23.75" customHeight="1" s="11">
       <c r="A23" s="15" t="n">
         <v>20</v>
       </c>
@@ -3083,8 +3117,10 @@
       <c r="C23" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="D23" s="24" t="b">
-        <v>1</v>
+      <c r="D23" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E23" s="24" t="n">
         <v>7</v>
@@ -3122,8 +3158,10 @@
           <t>random_oversample</t>
         </is>
       </c>
-      <c r="M23" s="23" t="b">
-        <v>1</v>
+      <c r="M23" s="25" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="N23" s="23" t="inlineStr">
         <is>
@@ -3185,20 +3223,22 @@
       </c>
       <c r="AD23" s="15" t="n"/>
     </row>
-    <row r="24" ht="12.8" customHeight="1" s="11">
+    <row r="24" ht="23.75" customHeight="1" s="11">
       <c r="A24" s="15" t="n">
         <v>21</v>
       </c>
       <c r="B24" s="15" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C24" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="D24" s="24" t="b">
-        <v>1</v>
+      <c r="D24" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E24" s="24" t="n">
         <v>7</v>
@@ -3236,8 +3276,10 @@
           <t>random_oversample</t>
         </is>
       </c>
-      <c r="M24" s="23" t="b">
-        <v>1</v>
+      <c r="M24" s="26" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="N24" s="23" t="inlineStr">
         <is>
@@ -3259,21 +3301,47 @@
           <t>GBC</t>
         </is>
       </c>
-      <c r="R24" s="15" t="n"/>
-      <c r="S24" s="15" t="n"/>
-      <c r="T24" s="15" t="n"/>
-      <c r="U24" s="15" t="n"/>
-      <c r="V24" s="15" t="n"/>
-      <c r="W24" s="15" t="n"/>
-      <c r="X24" s="15" t="n"/>
-      <c r="Y24" s="15" t="n"/>
-      <c r="Z24" s="15" t="n"/>
-      <c r="AA24" s="15" t="n"/>
-      <c r="AB24" s="15" t="n"/>
-      <c r="AC24" s="15" t="n"/>
+      <c r="R24" s="15" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="S24" s="15" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="T24" s="15" t="inlineStr">
+        <is>
+          <t>under-fitting (high bias and high variance)</t>
+        </is>
+      </c>
+      <c r="U24" s="15" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="V24" s="15" t="n">
+        <v>0.003252</v>
+      </c>
+      <c r="W24" s="15" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="X24" s="15" t="n">
+        <v>0.002949</v>
+      </c>
+      <c r="Y24" s="15" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="Z24" s="15" t="n">
+        <v>0.003613</v>
+      </c>
+      <c r="AA24" s="15" t="n">
+        <v>432.5</v>
+      </c>
+      <c r="AB24" s="15" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AC24" s="15" t="n">
+        <v>40836</v>
+      </c>
       <c r="AD24" s="15" t="n"/>
     </row>
-    <row r="25" ht="12.8" customHeight="1" s="11">
+    <row r="25" ht="23.75" customHeight="1" s="11">
       <c r="A25" s="15" t="n">
         <v>22</v>
       </c>
@@ -3285,8 +3353,10 @@
       <c r="C25" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="24" t="b">
-        <v>1</v>
+      <c r="D25" s="24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="E25" s="24" t="n">
         <v>7</v>
@@ -3324,8 +3394,10 @@
           <t>random_oversample</t>
         </is>
       </c>
-      <c r="M25" s="23" t="b">
-        <v>1</v>
+      <c r="M25" s="26" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="N25" s="23" t="inlineStr">
         <is>
@@ -3360,10 +3432,6 @@
       <c r="AB25" s="15" t="n"/>
       <c r="AC25" s="15" t="n"/>
       <c r="AD25" s="15" t="n"/>
-      <c r="AF25" s="10" t="n"/>
-      <c r="AG25" s="10" t="n"/>
-      <c r="AH25" s="10" t="n"/>
-      <c r="AI25" s="10" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
Version Nov 18, 2021
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/evaluation_output.xlsx
+++ b/data_driven/modeling/output/evaluation_output.xlsx
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -53,11 +53,6 @@
       <charset val="1"/>
       <family val="2"/>
       <color rgb="FF000000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -176,7 +171,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -201,10 +196,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -236,10 +231,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -605,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="H1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R25" activeCellId="0" sqref="R24:AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -3276,7 +3268,7 @@
           <t>random_oversample</t>
         </is>
       </c>
-      <c r="M24" s="26" t="inlineStr">
+      <c r="M24" s="23" t="inlineStr">
         <is>
           <t>True</t>
         </is>
@@ -3302,10 +3294,10 @@
         </is>
       </c>
       <c r="R24" s="15" t="n">
-        <v>0.28</v>
+        <v>0.57</v>
       </c>
       <c r="S24" s="15" t="n">
-        <v>0.51</v>
+        <v>0.61</v>
       </c>
       <c r="T24" s="15" t="inlineStr">
         <is>
@@ -3313,31 +3305,31 @@
         </is>
       </c>
       <c r="U24" s="15" t="n">
-        <v>0.55</v>
+        <v>0.43</v>
       </c>
       <c r="V24" s="15" t="n">
-        <v>0.003252</v>
+        <v>0.003374</v>
       </c>
       <c r="W24" s="15" t="n">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="X24" s="15" t="n">
-        <v>0.002949</v>
+        <v>0.003645</v>
       </c>
       <c r="Y24" s="15" t="n">
-        <v>0.62</v>
+        <v>0.78</v>
       </c>
       <c r="Z24" s="15" t="n">
-        <v>0.003613</v>
+        <v>0.002041</v>
       </c>
       <c r="AA24" s="15" t="n">
-        <v>432.5</v>
+        <v>1639.23</v>
       </c>
       <c r="AB24" s="15" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="AC24" s="15" t="n">
-        <v>40836</v>
+        <v>137601</v>
       </c>
       <c r="AD24" s="15" t="n"/>
     </row>
@@ -3394,7 +3386,7 @@
           <t>random_oversample</t>
         </is>
       </c>
-      <c r="M25" s="26" t="inlineStr">
+      <c r="M25" s="23" t="inlineStr">
         <is>
           <t>True</t>
         </is>

</xml_diff>

<commit_message>
Version Nov 19, 2021
</commit_message>
<xml_diff>
--- a/data_driven/modeling/output/evaluation_output.xlsx
+++ b/data_driven/modeling/output/evaluation_output.xlsx
@@ -957,7 +957,9 @@
       <c r="AC4" s="15" t="n">
         <v>134077</v>
       </c>
-      <c r="AD4" s="15" t="n"/>
+      <c r="AD4" s="15" t="n">
+        <v>7</v>
+      </c>
       <c r="AF4" s="22" t="n"/>
       <c r="AG4" s="15" t="inlineStr">
         <is>
@@ -1081,7 +1083,9 @@
       <c r="AC5" s="15" t="n">
         <v>135668</v>
       </c>
-      <c r="AD5" s="15" t="n"/>
+      <c r="AD5" s="15" t="n">
+        <v>4</v>
+      </c>
       <c r="AF5" s="21" t="n"/>
       <c r="AG5" s="15" t="inlineStr">
         <is>
@@ -1205,7 +1209,9 @@
       <c r="AC6" s="15" t="n">
         <v>136493</v>
       </c>
-      <c r="AD6" s="15" t="n"/>
+      <c r="AD6" s="15" t="n">
+        <v>4</v>
+      </c>
       <c r="AF6" s="23" t="n"/>
       <c r="AG6" s="15" t="inlineStr">
         <is>
@@ -1329,7 +1335,9 @@
       <c r="AC7" s="15" t="n">
         <v>138428</v>
       </c>
-      <c r="AD7" s="15" t="n"/>
+      <c r="AD7" s="15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" ht="23.85" customHeight="1" s="11">
       <c r="A8" s="15" t="n">
@@ -1447,7 +1455,9 @@
       <c r="AC8" s="15" t="n">
         <v>139142</v>
       </c>
-      <c r="AD8" s="15" t="n"/>
+      <c r="AD8" s="15" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" ht="23.85" customHeight="1" s="11">
       <c r="A9" s="15" t="n">
@@ -1565,7 +1575,9 @@
       <c r="AC9" s="15" t="n">
         <v>128165</v>
       </c>
-      <c r="AD9" s="15" t="n"/>
+      <c r="AD9" s="15" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" ht="23.85" customHeight="1" s="11">
       <c r="A10" s="15" t="n">
@@ -1683,7 +1695,9 @@
       <c r="AC10" s="15" t="n">
         <v>135593</v>
       </c>
-      <c r="AD10" s="15" t="n"/>
+      <c r="AD10" s="15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" ht="23.85" customHeight="1" s="11">
       <c r="A11" s="15" t="n">
@@ -1801,7 +1815,9 @@
       <c r="AC11" s="15" t="n">
         <v>136224</v>
       </c>
-      <c r="AD11" s="15" t="n"/>
+      <c r="AD11" s="15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" ht="23.85" customHeight="1" s="11">
       <c r="A12" s="15" t="n">
@@ -1919,7 +1935,9 @@
       <c r="AC12" s="15" t="n">
         <v>131538</v>
       </c>
-      <c r="AD12" s="15" t="n"/>
+      <c r="AD12" s="15" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" ht="23.85" customHeight="1" s="11">
       <c r="A13" s="15" t="n">
@@ -2035,7 +2053,9 @@
       <c r="AC13" s="15" t="n">
         <v>36003</v>
       </c>
-      <c r="AD13" s="15" t="n"/>
+      <c r="AD13" s="15" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" ht="23.85" customHeight="1" s="11">
       <c r="A14" s="15" t="n">
@@ -2151,7 +2171,9 @@
       <c r="AC14" s="15" t="n">
         <v>12931</v>
       </c>
-      <c r="AD14" s="15" t="n"/>
+      <c r="AD14" s="15" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" ht="23.85" customHeight="1" s="11">
       <c r="A15" s="15" t="n">
@@ -2269,7 +2291,9 @@
       <c r="AC15" s="15" t="n">
         <v>136006</v>
       </c>
-      <c r="AD15" s="15" t="n"/>
+      <c r="AD15" s="15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" ht="23.75" customHeight="1" s="11">
       <c r="A16" s="15" t="n">
@@ -2387,7 +2411,9 @@
       <c r="AC16" s="15" t="n">
         <v>137440</v>
       </c>
-      <c r="AD16" s="15" t="n"/>
+      <c r="AD16" s="15" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" ht="23.75" customHeight="1" s="11">
       <c r="A17" s="15" t="n">
@@ -2505,7 +2531,9 @@
       <c r="AC17" s="15" t="n">
         <v>136778</v>
       </c>
-      <c r="AD17" s="15" t="n"/>
+      <c r="AD17" s="15" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" ht="23.75" customHeight="1" s="11">
       <c r="A18" s="15" t="n">
@@ -2623,7 +2651,9 @@
       <c r="AC18" s="15" t="n">
         <v>21989</v>
       </c>
-      <c r="AD18" s="15" t="n"/>
+      <c r="AD18" s="15" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" ht="23.75" customHeight="1" s="11">
       <c r="A19" s="15" t="n">
@@ -2741,7 +2771,9 @@
       <c r="AC19" s="15" t="n">
         <v>21970</v>
       </c>
-      <c r="AD19" s="15" t="n"/>
+      <c r="AD19" s="15" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" ht="23.75" customHeight="1" s="11">
       <c r="A20" s="15" t="n">
@@ -2859,7 +2891,9 @@
       <c r="AC20" s="15" t="n">
         <v>138879</v>
       </c>
-      <c r="AD20" s="15" t="n"/>
+      <c r="AD20" s="15" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" ht="23.75" customHeight="1" s="11">
       <c r="A21" s="15" t="n">
@@ -2977,7 +3011,9 @@
       <c r="AC21" s="15" t="n">
         <v>137741</v>
       </c>
-      <c r="AD21" s="15" t="n"/>
+      <c r="AD21" s="15" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" ht="23.75" customHeight="1" s="11">
       <c r="A22" s="15" t="n">
@@ -3095,7 +3131,9 @@
       <c r="AC22" s="15" t="n">
         <v>138426</v>
       </c>
-      <c r="AD22" s="15" t="n"/>
+      <c r="AD22" s="15" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" ht="23.75" customHeight="1" s="11">
       <c r="A23" s="15" t="n">
@@ -3213,7 +3251,9 @@
       <c r="AC23" s="15" t="n">
         <v>135912</v>
       </c>
-      <c r="AD23" s="15" t="n"/>
+      <c r="AD23" s="15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" ht="23.75" customHeight="1" s="11">
       <c r="A24" s="15" t="n">
@@ -3331,7 +3371,9 @@
       <c r="AC24" s="15" t="n">
         <v>137601</v>
       </c>
-      <c r="AD24" s="15" t="n"/>
+      <c r="AD24" s="15" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" ht="23.75" customHeight="1" s="11">
       <c r="A25" s="15" t="n">
@@ -3339,7 +3381,7 @@
       </c>
       <c r="B25" s="15" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C25" s="15" t="n">
@@ -3411,19 +3453,47 @@
           <t>ANNC</t>
         </is>
       </c>
-      <c r="R25" s="15" t="n"/>
-      <c r="S25" s="15" t="n"/>
-      <c r="T25" s="15" t="n"/>
-      <c r="U25" s="15" t="n"/>
-      <c r="V25" s="15" t="n"/>
-      <c r="W25" s="15" t="n"/>
-      <c r="X25" s="15" t="n"/>
-      <c r="Y25" s="15" t="n"/>
-      <c r="Z25" s="15" t="n"/>
-      <c r="AA25" s="15" t="n"/>
-      <c r="AB25" s="15" t="n"/>
-      <c r="AC25" s="15" t="n"/>
-      <c r="AD25" s="15" t="n"/>
+      <c r="R25" s="15" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="S25" s="15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T25" s="15" t="inlineStr">
+        <is>
+          <t>under-fitting (high bias and high variance)</t>
+        </is>
+      </c>
+      <c r="U25" s="15" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="V25" s="15" t="n">
+        <v>0.003349</v>
+      </c>
+      <c r="W25" s="15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="X25" s="15" t="n">
+        <v>0.001403</v>
+      </c>
+      <c r="Y25" s="15" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="Z25" s="15" t="n">
+        <v>0.006131</v>
+      </c>
+      <c r="AA25" s="15" t="n">
+        <v>7942.58</v>
+      </c>
+      <c r="AB25" s="15" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="AC25" s="15" t="n">
+        <v>137427</v>
+      </c>
+      <c r="AD25" s="15" t="n">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>